<commit_message>
add lesson 24 tuvung
</commit_message>
<xml_diff>
--- a/TuVung/Lesson23/tuvung.xlsx
+++ b/TuVung/Lesson23/tuvung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_LearningJapaneseWebProject\TuVung\Lesson23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A5F6AF-E7E3-469F-902B-EB1D8364542D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F680F2CA-8398-4688-B475-3F35F1E32F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>cho, tặng</t>
   </si>
   <si>
-    <t>biết, tăng</t>
-  </si>
-  <si>
     <t>tiền bối, người đi trước</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>ハイヒール</t>
+  </si>
+  <si>
+    <t>biếu, tặng</t>
   </si>
 </sst>
 </file>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
@@ -746,7 +746,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -757,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
         <v>50</v>
@@ -768,7 +768,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -790,10 +790,10 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,7 +810,7 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
         <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +870,7 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
         <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -923,7 +923,7 @@
       </c>
       <c r="C21" s="5"/>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -947,15 +947,15 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -963,7 +963,7 @@
         <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -971,7 +971,7 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -1004,15 +1004,15 @@
         <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -1028,15 +1028,15 @@
         <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1044,15 +1044,15 @@
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>